<commit_message>
More report writing, fixed results, fixed lab3 file names to work in latex
</commit_message>
<xml_diff>
--- a/Lab3 (Constant Volatge Reference MPPT)/results_190827.xlsx
+++ b/Lab3 (Constant Volatge Reference MPPT)/results_190827.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Sync\Education\University\2019_Sem2(SPR)\48550 (Renewable Energy Systems)\Labs\Renewables\Lab3 (Constant Volatge Reference MPPT)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\12051342\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA68638-8146-46B0-AA5E-3E81E94C7EB7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="345" windowWidth="19185" windowHeight="10200" xr2:uid="{6CCD1161-8D19-4827-AEE4-517E09491DF5}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -51,7 +50,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -115,6 +114,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>I-V Curve of PV Emulator</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -243,40 +268,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>412</c:v>
+                  <c:v>0.41199999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>411</c:v>
+                  <c:v>0.41099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>411</c:v>
+                  <c:v>0.41099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>411</c:v>
+                  <c:v>0.41099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>410</c:v>
+                  <c:v>0.41</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>409</c:v>
+                  <c:v>0.40899999999999997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>396</c:v>
+                  <c:v>0.39600000000000002</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>313</c:v>
+                  <c:v>0.313</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>208</c:v>
+                  <c:v>0.20799999999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>95</c:v>
+                  <c:v>9.5000000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>85</c:v>
+                  <c:v>8.5000000000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>77</c:v>
+                  <c:v>7.6999999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>0</c:v>
@@ -323,6 +348,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Voltage (V)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -385,6 +466,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Current (A)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -436,6 +573,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -443,7 +581,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -493,6 +630,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>P-V Curve of PV Emulator</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -693,6 +856,67 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Voltage</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-AU" baseline="0"/>
+                  <a:t> (V)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-AU"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -755,6 +979,62 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Power (W)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -806,6 +1086,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -813,7 +1094,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -2333,11 +2613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB4A436E-AEB4-4ABA-A891-262A5E0286B6}">
-  <dimension ref="A1:D15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D15"/>
+      <selection activeCell="T25" sqref="T25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,12 +2625,12 @@
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>6.1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2364,42 +2644,50 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
       <c r="B3">
-        <v>412</v>
+        <v>0.41199999999999998</v>
       </c>
       <c r="C3">
         <v>0.22</v>
       </c>
       <c r="D3">
-        <f>C3*(B3/1000)</f>
+        <f>C3*B3</f>
         <v>9.0639999999999998E-2</v>
       </c>
+      <c r="E3">
+        <f>B3/1000</f>
+        <v>4.1199999999999999E-4</v>
+      </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>411</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="C4">
         <v>0.7</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:D15" si="0">C4*(B4/1000)</f>
+        <f t="shared" ref="D4:D15" si="0">C4*B4</f>
         <v>0.28769999999999996</v>
       </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E15" si="1">B4/1000</f>
+        <v>4.1099999999999996E-4</v>
+      </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4.7</v>
       </c>
       <c r="B5">
-        <v>411</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="C5">
         <v>2.17</v>
@@ -2408,13 +2696,17 @@
         <f t="shared" si="0"/>
         <v>0.89186999999999994</v>
       </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>4.1099999999999996E-4</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>10</v>
       </c>
       <c r="B6">
-        <v>411</v>
+        <v>0.41099999999999998</v>
       </c>
       <c r="C6">
         <v>4.34</v>
@@ -2423,13 +2715,17 @@
         <f t="shared" si="0"/>
         <v>1.7837399999999999</v>
       </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>4.1099999999999996E-4</v>
+      </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>22</v>
       </c>
       <c r="B7">
-        <v>410</v>
+        <v>0.41</v>
       </c>
       <c r="C7">
         <v>9</v>
@@ -2438,13 +2734,17 @@
         <f t="shared" si="0"/>
         <v>3.69</v>
       </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>4.0999999999999999E-4</v>
+      </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>33</v>
       </c>
       <c r="B8">
-        <v>409</v>
+        <v>0.40899999999999997</v>
       </c>
       <c r="C8">
         <v>13.3</v>
@@ -2453,13 +2753,17 @@
         <f t="shared" si="0"/>
         <v>5.4397000000000002</v>
       </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>4.0899999999999997E-4</v>
+      </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>47</v>
       </c>
       <c r="B9">
-        <v>396</v>
+        <v>0.39600000000000002</v>
       </c>
       <c r="C9">
         <v>18.5</v>
@@ -2468,13 +2772,17 @@
         <f t="shared" si="0"/>
         <v>7.3260000000000005</v>
       </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>3.9600000000000003E-4</v>
+      </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>68</v>
       </c>
       <c r="B10">
-        <v>313</v>
+        <v>0.313</v>
       </c>
       <c r="C10">
         <v>20.9</v>
@@ -2483,13 +2791,17 @@
         <f t="shared" si="0"/>
         <v>6.5416999999999996</v>
       </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>3.1300000000000002E-4</v>
+      </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>100</v>
       </c>
       <c r="B11">
-        <v>208</v>
+        <v>0.20799999999999999</v>
       </c>
       <c r="C11">
         <v>20.9</v>
@@ -2498,13 +2810,17 @@
         <f t="shared" si="0"/>
         <v>4.3471999999999991</v>
       </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>2.0799999999999999E-4</v>
+      </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>220</v>
       </c>
       <c r="B12">
-        <v>95</v>
+        <v>9.5000000000000001E-2</v>
       </c>
       <c r="C12">
         <v>20.9</v>
@@ -2513,13 +2829,17 @@
         <f t="shared" si="0"/>
         <v>1.9854999999999998</v>
       </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>9.5000000000000005E-5</v>
+      </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>245</v>
       </c>
       <c r="B13">
-        <v>85</v>
+        <v>8.5000000000000006E-2</v>
       </c>
       <c r="C13">
         <v>20.9</v>
@@ -2528,13 +2848,17 @@
         <f t="shared" si="0"/>
         <v>1.7765</v>
       </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>8.5000000000000006E-5</v>
+      </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>270</v>
       </c>
       <c r="B14">
-        <v>77</v>
+        <v>7.6999999999999999E-2</v>
       </c>
       <c r="C14">
         <v>20.9</v>
@@ -2543,8 +2867,12 @@
         <f t="shared" si="0"/>
         <v>1.6093</v>
       </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>7.7000000000000001E-5</v>
+      </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -2556,6 +2884,10 @@
       </c>
       <c r="D15">
         <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>